<commit_message>
Official Proceeding more or less complete
</commit_message>
<xml_diff>
--- a/pisar/data/personnel-demo.xlsx
+++ b/pisar/data/personnel-demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B31EEF8-8A2C-4B80-B34A-670F5DB739E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8AB210-74F2-425E-BD21-67F83B9578B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>№
 п/п</t>
@@ -230,6 +230,24 @@
   </si>
   <si>
     <t>19.6.1988</t>
+  </si>
+  <si>
+    <t>Даутов Искандер Садыкович</t>
+  </si>
+  <si>
+    <t>Говоров Леонид Александрович</t>
+  </si>
+  <si>
+    <t>Командир роты</t>
+  </si>
+  <si>
+    <t>заместитель командира роты по военно-политической работе</t>
+  </si>
+  <si>
+    <t>06.04.1967</t>
+  </si>
+  <si>
+    <t>31.03.1971</t>
   </si>
 </sst>
 </file>
@@ -652,16 +670,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ11"/>
+  <dimension ref="A1:AZ8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.06640625" customWidth="1"/>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.73046875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="22.53125" customWidth="1"/>
     <col min="5" max="5" width="20.9296875" customWidth="1"/>
@@ -859,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
@@ -882,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -908,7 +926,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -957,7 +975,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -983,13 +1001,25 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.45">
@@ -997,55 +1027,25 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full text for company, platoon...
</commit_message>
<xml_diff>
--- a/pisar/data/personnel-demo.xlsx
+++ b/pisar/data/personnel-demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA70BBB-8540-4A3A-8406-E6256045DFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1014BB0E-8F73-4910-A789-B6EE9D0658BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>№
 п/п</t>
@@ -277,13 +277,43 @@
   </si>
   <si>
     <t>ЖЗ-766212</t>
+  </si>
+  <si>
+    <t>3 отделение</t>
+  </si>
+  <si>
+    <t>1 стрелковая рота</t>
+  </si>
+  <si>
+    <t>3 разведывательная рота</t>
+  </si>
+  <si>
+    <t>2 стрелковый взвод</t>
+  </si>
+  <si>
+    <t>3 разведывательный взвод</t>
+  </si>
+  <si>
+    <t>2 артиллерийская рота</t>
+  </si>
+  <si>
+    <t>1 артиллерийская батарея</t>
+  </si>
+  <si>
+    <t>2 орудийный расчет</t>
+  </si>
+  <si>
+    <t>4 разведывательное отделение</t>
+  </si>
+  <si>
+    <t>Наводчик</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +356,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -714,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -916,14 +952,14 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
@@ -945,17 +981,17 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="M3" t="s">
         <v>54</v>
@@ -974,14 +1010,14 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
       </c>
       <c r="F4" t="s">
         <v>52</v>
@@ -1156,6 +1192,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new utility for sorting
</commit_message>
<xml_diff>
--- a/pisar/data/personnel-demo.xlsx
+++ b/pisar/data/personnel-demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455F35AA-DD6E-4513-8BCD-4C639F6B9308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4535500A-B22A-446D-B14A-913A7ACA6954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
   <si>
     <t>№
 п/п</t>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>ЛК-884912</t>
+  </si>
+  <si>
+    <t>РЦ-365212</t>
   </si>
 </sst>
 </file>
@@ -753,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,6 +1089,9 @@
       <c r="M6" t="s">
         <v>54</v>
       </c>
+      <c r="N6" t="s">
+        <v>92</v>
+      </c>
       <c r="O6" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
current progress in Official Proceeding
</commit_message>
<xml_diff>
--- a/pisar/data/personnel-demo.xlsx
+++ b/pisar/data/personnel-demo.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05B8CA5-DEB8-42F4-A266-F4DF4A1ECCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A2DBA4-FD7A-4958-A89C-32DF4F740DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>ЖЗ-766212</t>
   </si>
   <si>
-    <t>3 отделение</t>
-  </si>
-  <si>
     <t>1 стрелковая рота</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>РЦ-365212</t>
+  </si>
+  <si>
+    <t>3 стрелковое отделение</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   <dimension ref="A1:BA10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -959,13 +959,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
@@ -988,16 +988,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
         <v>86</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>87</v>
       </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M3" t="s">
         <v>54</v>
@@ -1017,13 +1017,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
         <v>52</v>
@@ -1061,7 +1061,7 @@
         <v>53</v>
       </c>
       <c r="N5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O5" t="s">
         <v>71</v>
@@ -1090,7 +1090,7 @@
         <v>54</v>
       </c>
       <c r="N6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O6" t="s">
         <v>63</v>

</xml_diff>